<commit_message>
Aggiornato file con indicazioni richieste
</commit_message>
<xml_diff>
--- a/GATEWAY/A1111DSPSRLXXXXX/DSP/HCSuite/v4.3.0/report-checklist.xlsx
+++ b/GATEWAY/A1111DSPSRLXXXXX/DSP/HCSuite/v4.3.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele Santonastaso\Documents\Work\DSP\FSE20\DSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47646ECD-B2D5-4D9C-B796-B7115134986A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B89DBF-E9A5-46D4-9AF5-1BA225D89B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="885">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4599,9 +4599,6 @@
     <t>1805537544a08d7c</t>
   </si>
   <si>
-    <t>per HCSUITE i nome del paziente è obbligatorio</t>
-  </si>
-  <si>
     <t>c6c5e36a4c9019d2</t>
   </si>
   <si>
@@ -4618,9 +4615,6 @@
     <t>HCSUITE non gestisce l'inserimento nel documento di tutte le section opzionali.</t>
   </si>
   <si>
-    <t>per HCSUITE il sesso del paziente è codificato pertanto non sarebbe possibile avere una codifica sbaglaita</t>
-  </si>
-  <si>
     <t>4b636ccc9edd607c</t>
   </si>
   <si>
@@ -4654,6 +4648,14 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.30.4.4.f73c310a2f47b46ae8bc97415654396ee27a50900657b4ae46c94ce9a55eb331.4a233fc53d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>HCSUITE dispone di un modulo, integrato con l'anagrafica centralizzata che permette all'operatore abilitato di valorizzare il campo relativo ai dati anagrafici del paziente</t>
+  </si>
+  <si>
+    <t>HCSUITE inserisce il valore dell'NRE nel tag 	
+&lt;inFulfillmentOf typeCode="FLFS"&gt;
+solo se presente, in caso contrario non genera il TAG</t>
   </si>
 </sst>
 </file>
@@ -7571,10 +7573,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K169" sqref="A1:T1000"/>
+      <selection pane="bottomRight" activeCell="K166" sqref="K166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -12862,7 +12864,7 @@
         <v>847</v>
       </c>
       <c r="K156" s="25" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -12900,7 +12902,7 @@
         <v>847</v>
       </c>
       <c r="K157" s="34" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -12991,7 +12993,7 @@
         <v>138</v>
       </c>
       <c r="N159" s="25" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>138</v>
@@ -13072,7 +13074,7 @@
         <v>867</v>
       </c>
       <c r="I161" s="24" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J161" s="25" t="s">
         <v>138</v>
@@ -13084,14 +13086,18 @@
       <c r="M161" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="N161" s="25"/>
+      <c r="N161" s="25" t="s">
+        <v>875</v>
+      </c>
       <c r="O161" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P161" s="25"/>
+      <c r="P161" s="25" t="s">
+        <v>883</v>
+      </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26"/>
-      <c r="S161" s="37"/>
+      <c r="S161" s="34"/>
       <c r="T161" s="28" t="s">
         <v>104</v>
       </c>
@@ -13119,22 +13125,30 @@
         <v>45327.399293981478</v>
       </c>
       <c r="H162" s="24" t="s">
+        <v>868</v>
+      </c>
+      <c r="I162" s="24" t="s">
         <v>869</v>
-      </c>
-      <c r="I162" s="24" t="s">
-        <v>870</v>
       </c>
       <c r="J162" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K162" s="25" t="s">
-        <v>868</v>
-      </c>
-      <c r="L162" s="25"/>
-      <c r="M162" s="25"/>
-      <c r="N162" s="25"/>
-      <c r="O162" s="25"/>
-      <c r="P162" s="25"/>
+      <c r="K162" s="25"/>
+      <c r="L162" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="M162" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="N162" s="25" t="s">
+        <v>875</v>
+      </c>
+      <c r="O162" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="P162" s="25" t="s">
+        <v>883</v>
+      </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26"/>
       <c r="S162" s="37" t="s">
@@ -13167,17 +13181,15 @@
         <v>45327.653645833336</v>
       </c>
       <c r="H163" s="24" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="I163" s="24" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="J163" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K163" s="25" t="s">
-        <v>873</v>
-      </c>
+      <c r="K163" s="25"/>
       <c r="L163" s="25" t="s">
         <v>138</v>
       </c>
@@ -13185,12 +13197,14 @@
         <v>138</v>
       </c>
       <c r="N163" s="25" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="O163" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P163" s="25"/>
+      <c r="P163" s="25" t="s">
+        <v>883</v>
+      </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
       <c r="S163" s="27" t="s">
@@ -13224,7 +13238,7 @@
         <v>847</v>
       </c>
       <c r="K164" s="25" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -13262,7 +13276,7 @@
         <v>847</v>
       </c>
       <c r="K165" s="25" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="L165" s="25"/>
       <c r="M165" s="25"/>
@@ -13299,7 +13313,9 @@
       <c r="J166" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K166" s="25"/>
+      <c r="K166" s="25" t="s">
+        <v>884</v>
+      </c>
       <c r="L166" s="25"/>
       <c r="M166" s="25"/>
       <c r="N166" s="25"/>
@@ -13374,7 +13390,7 @@
         <v>847</v>
       </c>
       <c r="K168" s="25" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="L168" s="25"/>
       <c r="M168" s="25"/>
@@ -13412,7 +13428,7 @@
         <v>847</v>
       </c>
       <c r="K169" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -13488,7 +13504,7 @@
         <v>847</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -13526,7 +13542,7 @@
         <v>847</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -13564,7 +13580,7 @@
         <v>847</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -13602,7 +13618,7 @@
         <v>847</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -13640,7 +13656,7 @@
         <v>847</v>
       </c>
       <c r="K175" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>
@@ -13678,7 +13694,7 @@
         <v>847</v>
       </c>
       <c r="K176" s="25" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="L176" s="25"/>
       <c r="M176" s="25"/>
@@ -20651,10 +20667,10 @@
         <v>45328.490266203706</v>
       </c>
       <c r="H381" s="35" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="I381" s="35" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="J381" s="25" t="s">
         <v>138</v>
@@ -25418,7 +25434,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>

</xml_diff>

<commit_message>
Fornitore A1111DSPSRLXXXXX - DSP - HCSuite - v4.3.0 - CASO ID:48
Nuova sottomissione checklist dettagliando il comportamento per il caso ID:48
</commit_message>
<xml_diff>
--- a/GATEWAY/A1111DSPSRLXXXXX/DSP/HCSuite/v4.3.0/report-checklist.xlsx
+++ b/GATEWAY/A1111DSPSRLXXXXX/DSP/HCSuite/v4.3.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele Santonastaso\Documents\Work\DSP\FSE20\DSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B89DBF-E9A5-46D4-9AF5-1BA225D89B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DDF4E8-5F73-402F-B2F2-7954812CD979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="886">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4565,11 +4565,6 @@
 </t>
   </si>
   <si>
-    <t>All'interno della configurazine di HCSUITE c'è una proprietà che indica come il sistema si deve comportare in caso si questo errore.
-Se il parametro è impostato a true allora il sistema ignora l'errore e procede con la firma e il processo continua normalmente.
-Se invece ila proprietà è false il sistema si blocca e permetre al medico di riprovare ad inviare il documento in validazione</t>
-  </si>
-  <si>
     <t>Errore nella validazione del CDA2: timeout nella chiamata al gateway FSE</t>
   </si>
   <si>
@@ -4582,21 +4577,6 @@
   </si>
   <si>
     <t>1095a64117ef0704</t>
-  </si>
-  <si>
-    <t>{
-  "traceID": "1095a64117ef0704",
-  "spanID": "1095a64117ef0704",
-  "type": "/msg/jwt-validation",
-  "title": "Campo token JWT non valido.",
-  "detail": "Il codice fiscale nel campo person_id non è corretto",
-  "status": 403,
-  "instance": "/jwt-mandatory-field-malformed",
-  "workflowInstanceId": "UNKNOWN_WORKFLOW_ID"
-}</t>
-  </si>
-  <si>
-    <t>1805537544a08d7c</t>
   </si>
   <si>
     <t>c6c5e36a4c9019d2</t>
@@ -4621,10 +4601,6 @@
     <t>2.16.840.1.113883.2.9.2.30.4.4.94108b233c89416717b3298248d4e85bb35251778ae64c27e4e71e444698965a.50c52a723f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">  "2.16.840.1.113883.2.9.2.30.4.4.fa2a0a21161dd2a1d63f2f8e6b5783db19749ef10493400f374d2f2cca149581.6fc2d1c55b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
-</t>
-  </si>
-  <si>
     <t>"Errore durante la validazione del documento per il fascicolo sanitario." + la descrizione dell'errore ritornata dal gateway</t>
   </si>
   <si>
@@ -4656,6 +4632,28 @@
     <t>HCSUITE inserisce il valore dell'NRE nel tag 	
 &lt;inFulfillmentOf typeCode="FLFS"&gt;
 solo se presente, in caso contrario non genera il TAG</t>
+  </si>
+  <si>
+    <t>"UNKNOWN_WORKFLOW_ID"</t>
+  </si>
+  <si>
+    <t>L'applicativo può essere configurato per comportarsi nei seguenti modi a seconda delle disposizioni regionali e delle scelte aziendali:
+1. L'errore è bloccante e il referto torna in coda di firma. Dopo che l'errore è stato corretto dal medico o dal personale amministrativo, il referto può essere firmato nuovamente e inviato al respoitory aziendale  che si occuperà dell'invio a FSE o al middelware regionale che invierà il documento al FSE.
+2. Il referto viene comunque firmato e inviato al repository aziendale per la consegna al paziente e la consultazione interna. Una volta corretto l'errore,  il medico può  generare e firmare un referto sostitutivo e archiviarlo su respoitory aziendale che si occuperà dell'invio a FSE o al middelware regionale che invierà il documento al FSE..
+HCSUITE dispone di un modulo, integrato con l'anagrafica centralizzata che permette all'operatore abilitato di valorizzare il campo relativo ai dati anagrafici del paziente</t>
+  </si>
+  <si>
+    <t>f995018286f786cf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.450f8bb2afeb8259d4e15b7d5ac1266bc122025ef0f89be954f0115226ce30b4.a88961f3f2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>All'interno della configurazine di HCSUITE c'è una proprietà che indica come il sistema si deve comportare in caso si questo errore.
+Tramite questo parametro è possibile configurare l'applicativo per operare in diverse modalità in base alle normative regionali e alle decisioni aziendali:
+1. Se il parametro è impostato a "false", il referto viene messo in coda per la firma. Il medico ha la possibilità di ripetere la firma; se questa ha successo, il documento viene archiviato nel repository aziendale per l'invio al Fascicolo Sanitario Elettronico (FSE) o al middleware regionale, che provvederà a inoltrarlo al FSE.
+2. Se il parametro è impostao a "true" Il referto viene comunque firmato e inviato al repository aziendale per la distribuzione al paziente e la consultazione interna. Successivamente, il medico può generare e firmare un referto sostitutivo, che sarà anch'esso archiviato nel repository aziendale per l'invio al FSE o al middleware regionale, che si occuperà di trasmetterlo al FSE.
+In ogni caso tutte le informazioni vengono scritte in un file di log e messe a disposizione degli amministratori</t>
   </si>
 </sst>
 </file>
@@ -7573,10 +7571,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K166" sqref="K166"/>
+      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9409,13 +9407,13 @@
         <v>847</v>
       </c>
       <c r="N55" s="34" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="O55" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P55" s="34" t="s">
-        <v>861</v>
+        <v>885</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -12788,7 +12786,7 @@
         <v>847</v>
       </c>
       <c r="K154" s="34" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="L154" s="25"/>
       <c r="M154" s="25"/>
@@ -12826,7 +12824,7 @@
         <v>847</v>
       </c>
       <c r="K155" s="25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -12864,7 +12862,7 @@
         <v>847</v>
       </c>
       <c r="K156" s="25" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -12902,7 +12900,7 @@
         <v>847</v>
       </c>
       <c r="K157" s="34" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -12977,10 +12975,10 @@
         <v>45327.384791666664</v>
       </c>
       <c r="H159" s="35" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I159" s="36" t="s">
-        <v>866</v>
+        <v>881</v>
       </c>
       <c r="J159" s="25" t="s">
         <v>138</v>
@@ -12993,7 +12991,7 @@
         <v>138</v>
       </c>
       <c r="N159" s="25" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>138</v>
@@ -13048,7 +13046,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="240.75" thickBot="1">
+    <row r="161" spans="1:20" ht="330.75" thickBot="1">
       <c r="A161" s="20">
         <v>154</v>
       </c>
@@ -13065,16 +13063,16 @@
         <v>351</v>
       </c>
       <c r="F161" s="23">
-        <v>45327</v>
+        <v>45334</v>
       </c>
       <c r="G161" s="24">
-        <v>45327.389733796299</v>
+        <v>45334.459363425929</v>
       </c>
       <c r="H161" s="24" t="s">
-        <v>867</v>
+        <v>883</v>
       </c>
       <c r="I161" s="24" t="s">
-        <v>874</v>
+        <v>884</v>
       </c>
       <c r="J161" s="25" t="s">
         <v>138</v>
@@ -13084,16 +13082,16 @@
         <v>847</v>
       </c>
       <c r="M161" s="25" t="s">
-        <v>847</v>
+        <v>138</v>
       </c>
       <c r="N161" s="25" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="O161" s="25" t="s">
         <v>138</v>
       </c>
       <c r="P161" s="25" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26"/>
@@ -13125,10 +13123,10 @@
         <v>45327.399293981478</v>
       </c>
       <c r="H162" s="24" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="I162" s="24" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="J162" s="25" t="s">
         <v>138</v>
@@ -13141,13 +13139,13 @@
         <v>138</v>
       </c>
       <c r="N162" s="25" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="O162" s="25" t="s">
         <v>138</v>
       </c>
       <c r="P162" s="25" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26"/>
@@ -13181,10 +13179,10 @@
         <v>45327.653645833336</v>
       </c>
       <c r="H163" s="24" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="I163" s="24" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="J163" s="25" t="s">
         <v>138</v>
@@ -13197,13 +13195,13 @@
         <v>138</v>
       </c>
       <c r="N163" s="25" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="O163" s="25" t="s">
         <v>138</v>
       </c>
       <c r="P163" s="25" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
@@ -13238,7 +13236,7 @@
         <v>847</v>
       </c>
       <c r="K164" s="25" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -13276,7 +13274,7 @@
         <v>847</v>
       </c>
       <c r="K165" s="25" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="L165" s="25"/>
       <c r="M165" s="25"/>
@@ -13314,7 +13312,7 @@
         <v>847</v>
       </c>
       <c r="K166" s="25" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L166" s="25"/>
       <c r="M166" s="25"/>
@@ -13390,7 +13388,7 @@
         <v>847</v>
       </c>
       <c r="K168" s="25" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="L168" s="25"/>
       <c r="M168" s="25"/>
@@ -13428,7 +13426,7 @@
         <v>847</v>
       </c>
       <c r="K169" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -13504,7 +13502,7 @@
         <v>847</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -13542,7 +13540,7 @@
         <v>847</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -13580,7 +13578,7 @@
         <v>847</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -13618,7 +13616,7 @@
         <v>847</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -13656,7 +13654,7 @@
         <v>847</v>
       </c>
       <c r="K175" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>
@@ -13694,7 +13692,7 @@
         <v>847</v>
       </c>
       <c r="K176" s="25" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="L176" s="25"/>
       <c r="M176" s="25"/>
@@ -20667,10 +20665,10 @@
         <v>45328.490266203706</v>
       </c>
       <c r="H381" s="35" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="I381" s="35" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="J381" s="25" t="s">
         <v>138</v>

</xml_diff>